<commit_message>
Compatibilização com novo formato da base da ANEEL
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2024/nomes_dist_powerbi.xlsx
+++ b/inst/dados_premissas/2024/nomes_dist_powerbi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos_r\epe4md\inst\dados_premissas\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PLAN26-30\dados_premissas\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C41FEA-300A-4C31-A39D-39C956074FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58DD0E9-FF03-4D47-8812-DCA98A11A3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="149">
   <si>
     <t>sig_agente</t>
   </si>
@@ -474,6 +474,15 @@
   </si>
   <si>
     <t>CERIPa</t>
+  </si>
+  <si>
+    <t>BOA VISTA</t>
+  </si>
+  <si>
+    <t>CERAL ARARUAMA</t>
+  </si>
+  <si>
+    <t>CERSAD DISTRIBUI</t>
   </si>
 </sst>
 </file>
@@ -835,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,6 +1918,54 @@
         <v>107</v>
       </c>
     </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>109</v>
+      </c>
+      <c r="B134" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>120</v>
+      </c>
+      <c r="B135" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>105</v>
+      </c>
+      <c r="B136" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>146</v>
+      </c>
+      <c r="B137" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>147</v>
+      </c>
+      <c r="B138" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>148</v>
+      </c>
+      <c r="B139" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B114" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>